<commit_message>
Proofreading through purple, page 22.
</commit_message>
<xml_diff>
--- a/TODO/Proofreading.xlsx
+++ b/TODO/Proofreading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="162">
   <si>
     <t>Page</t>
   </si>
@@ -282,6 +282,228 @@
   </si>
   <si>
     <t>Change text to this wording &lt;----</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Ordinary speech." </t>
+  </si>
+  <si>
+    <t>Decapatalize. Consider removing quotes.</t>
+  </si>
+  <si>
+    <t>Interaction</t>
+  </si>
+  <si>
+    <t>Is the last bullet necessary? I'm torn. Use your discretion.</t>
+  </si>
+  <si>
+    <t>Chemistry Text Box</t>
+  </si>
+  <si>
+    <t>Add that attack rolls should use either the Chemistry skill or, if thrown, the Ranged skill.</t>
+  </si>
+  <si>
+    <t>Block box</t>
+  </si>
+  <si>
+    <t>Change STR to Strength. Twice.</t>
+  </si>
+  <si>
+    <t>Block Box</t>
+  </si>
+  <si>
+    <t>Also modifier, not mod</t>
+  </si>
+  <si>
+    <t>Light armor box, 25 benefit: Add "This bonus can be used after the check has been made."</t>
+  </si>
+  <si>
+    <t>Medicine bullet points. Either remove "in combat" from "Heal an ally in combat" or merge it into first aid and remove a bullet.</t>
+  </si>
+  <si>
+    <t>Melee weapon 25 bonus</t>
+  </si>
+  <si>
+    <t>Change to When you score a critical hit…</t>
+  </si>
+  <si>
+    <t>Melee weapon 50 bonus</t>
+  </si>
+  <si>
+    <t>Melee weapon 75 bonus</t>
+  </si>
+  <si>
+    <t>Melee weapon boxes</t>
+  </si>
+  <si>
+    <t>This replaces the previous perk. Change wording to this.</t>
+  </si>
+  <si>
+    <t>Nature bullets</t>
+  </si>
+  <si>
+    <t>weird line break after mushrooms. Remove.</t>
+  </si>
+  <si>
+    <t>Magic textbox</t>
+  </si>
+  <si>
+    <t>The word magic here: Change to the word magic in this book</t>
+  </si>
+  <si>
+    <t>Ranged bullets: Throwing grabbed enemies/objects</t>
+  </si>
+  <si>
+    <t>change to enemies or objects</t>
+  </si>
+  <si>
+    <t>Ranged 25,50,75</t>
+  </si>
+  <si>
+    <t>Change on a critical hit to when you score a critical hit with a ranged weapon</t>
+  </si>
+  <si>
+    <t>Ranged, Melee bonus boxes</t>
+  </si>
+  <si>
+    <t>Make it so they can choose: Melee can choose prone, slow,  then prone, slow, stun. Ranged 75 can choose slow, CA or stunned.</t>
+  </si>
+  <si>
+    <t>Restoration: Change actual mod to Restoration modifier</t>
+  </si>
+  <si>
+    <t>Twice</t>
+  </si>
+  <si>
+    <t>Lockpick 25</t>
+  </si>
+  <si>
+    <t>Change to "Once per day, you can use your Security score in place of your Stealth score when making a check."</t>
+  </si>
+  <si>
+    <t>Lockpick 50</t>
+  </si>
+  <si>
+    <t>When attacking enemies you are hidden from, increase your damage die by one.</t>
+  </si>
+  <si>
+    <t>Emulate the language above, but two.</t>
+  </si>
+  <si>
+    <t>Custom skills: …Decide which Attribute</t>
+  </si>
+  <si>
+    <t>Does Attribute need to be capatalized?</t>
+  </si>
+  <si>
+    <t>We call them teir bonuses. I think the official language is "Skill Perks."</t>
+  </si>
+  <si>
+    <t>3 times in this paragraph.</t>
+  </si>
+  <si>
+    <t>Stacking bonuses</t>
+  </si>
+  <si>
+    <t>Capatalize Injure when Carmellia casts it.</t>
+  </si>
+  <si>
+    <t>…The monster would take both damage-&gt; Change to the monster would take damage from both attacks.</t>
+  </si>
+  <si>
+    <t>equipment… such as a stop sign or mailbox for a large character</t>
+  </si>
+  <si>
+    <t>Add a comma after character</t>
+  </si>
+  <si>
+    <t>weapons first paragraph</t>
+  </si>
+  <si>
+    <t>Also add that any weapon can be used one- or two-handed, modifying the damage die accordingly.</t>
+  </si>
+  <si>
+    <t>Permafrost spell thrice a day might be at low levels</t>
+  </si>
+  <si>
+    <t>Change to "might be for inexperienced adventurers."</t>
+  </si>
+  <si>
+    <t>Augments in your campaign… change curses to curse, and artifacts to an artifact.</t>
+  </si>
+  <si>
+    <t>"Even granting penalties or a mix or bonuses and penalties…</t>
+  </si>
+  <si>
+    <t>Change to "Even granting penalties, or a mix of bonuses and penalties…"</t>
+  </si>
+  <si>
+    <t>or maybe crafted standard projects</t>
+  </si>
+  <si>
+    <t>change to crafted as standard projects</t>
+  </si>
+  <si>
+    <t>GMs should be free</t>
+  </si>
+  <si>
+    <t>change to GMs should feel free</t>
+  </si>
+  <si>
+    <t>braces of calling</t>
+  </si>
+  <si>
+    <t>change to a pair of bracers of calling</t>
+  </si>
+  <si>
+    <t>Remove Alteration +5 from the table.</t>
+  </si>
+  <si>
+    <t>make sure we discuss encounter/day</t>
+  </si>
+  <si>
+    <t>Remove Restoration +5 from table</t>
+  </si>
+  <si>
+    <t>Make sure that ongoing damage is synonymous with (save ends)</t>
+  </si>
+  <si>
+    <t>Armor, re: kitten armor</t>
+  </si>
+  <si>
+    <t>Capatalize Stealth</t>
+  </si>
+  <si>
+    <t>…matter what is used, all items function..</t>
+  </si>
+  <si>
+    <t>change to a semicolon</t>
+  </si>
+  <si>
+    <t>Discus with a GM</t>
+  </si>
+  <si>
+    <t>Change to Discuss with your GM</t>
+  </si>
+  <si>
+    <t>Fortitude</t>
+  </si>
+  <si>
+    <t>Fortitude is character's ability to… change to a character's ability</t>
+  </si>
+  <si>
+    <t>Enlightenment table, column 45 should be +5 to attack rolls</t>
+  </si>
+  <si>
+    <t>This will have to change on the character sheet as well. Sorry!</t>
+  </si>
+  <si>
+    <t>Devout follower. 5 Enlightenment points is garbale. Can we make this 10?</t>
+  </si>
+  <si>
+    <t>For example, activating +2 damage…</t>
+  </si>
+  <si>
+    <t>Change +2 damage to Increase +2 Movement, and change ten points to fifteen (both times in this paragraph)</t>
   </si>
 </sst>
 </file>
@@ -635,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -856,7 +1078,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1173,186 +1395,468 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>14</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>14</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>14</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>12</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
+      <c r="A56">
+        <v>12</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>15</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
+    <row r="58" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>15</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>16</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>16</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>16</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>16</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>16</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>16</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>17</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>17</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>17</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>18</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>18</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>18</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>18</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>18</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>18</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>19</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>19</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="2"/>
+    <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>19</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>19</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>19</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>19</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="C84" s="2"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="2"/>
+    <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="C85" s="2"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
+    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>20</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="C86" s="2"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
+    <row r="87" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="C87" s="2"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="2"/>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>20</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>20</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>20</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>20</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>21</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>23</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>21</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>

</xml_diff>

<commit_message>
Proofread through talents. Page 31.
</commit_message>
<xml_diff>
--- a/TODO/Proofreading.xlsx
+++ b/TODO/Proofreading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="253">
   <si>
     <t>Page</t>
   </si>
@@ -504,6 +504,283 @@
   </si>
   <si>
     <t>Change +2 damage to Increase +2 Movement, and change ten points to fifteen (both times in this paragraph)</t>
+  </si>
+  <si>
+    <t>Defensive Disarming</t>
+  </si>
+  <si>
+    <t>Change Blocking to Block (Just on the capital one)</t>
+  </si>
+  <si>
+    <t>Defensive Warrior</t>
+  </si>
+  <si>
+    <t>Formatting on the prereqs is goof</t>
+  </si>
+  <si>
+    <t>Devoted Hunter Commanding presence is weirdly spaced</t>
+  </si>
+  <si>
+    <t>Dodging Adept</t>
+  </si>
+  <si>
+    <t>Add a period to the end.. Also on Devastating Block. And disciple of restoration</t>
+  </si>
+  <si>
+    <t>Fearful presence</t>
+  </si>
+  <si>
+    <t>Add a period to the end.</t>
+  </si>
+  <si>
+    <t>Duelist</t>
+  </si>
+  <si>
+    <t>Change "To the attack roll" to "To Melee Weapon attack rolls"</t>
+  </si>
+  <si>
+    <t>Tricky Steps</t>
+  </si>
+  <si>
+    <t>Add a period to the end</t>
+  </si>
+  <si>
+    <t>Quick Steps</t>
+  </si>
+  <si>
+    <t>Raised by the blind</t>
+  </si>
+  <si>
+    <t>Powrful Strike I-V</t>
+  </si>
+  <si>
+    <t>Far Shot</t>
+  </si>
+  <si>
+    <t>Capatalize Range</t>
+  </si>
+  <si>
+    <t>Fortune's Child</t>
+  </si>
+  <si>
+    <t>Change to: After rolling any die, you may spend two Fortune points to re-roll that die. You must take the second result.</t>
+  </si>
+  <si>
+    <t>Make sure it's stylized consistantly as Fortune points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unless a better style is better. I don't care, as long as it's consistent. </t>
+  </si>
+  <si>
+    <t>Derived attributes</t>
+  </si>
+  <si>
+    <t>decapatalize Magic</t>
+  </si>
+  <si>
+    <t>Heightened healing</t>
+  </si>
+  <si>
+    <t>rewrite: You know the location of all creatues within 5 squres of you. Treat the creatures as being fully seen by you when determining combat advantage and concealment.
+Or delete this Talent; it's pretty complex. Your call.</t>
+  </si>
+  <si>
+    <t>Improvised Weapoon Expert</t>
+  </si>
+  <si>
+    <t>Greater Shifting, healing fighter, Improvised  weapon expert</t>
+  </si>
+  <si>
+    <t>Change do to deal</t>
+  </si>
+  <si>
+    <t>Iron Resolve, Improvised Weapon Master, Improvised Weapon Handler</t>
+  </si>
+  <si>
+    <t>Iron Resolve</t>
+  </si>
+  <si>
+    <t>Capatalize Will</t>
+  </si>
+  <si>
+    <t>Lucky Block</t>
+  </si>
+  <si>
+    <t>Capatalize Block. Also add "This can be done after the roll has been made."</t>
+  </si>
+  <si>
+    <t>Gert rid of Improved Block; it no longer exists</t>
+  </si>
+  <si>
+    <t>Do we have rules for dual wielding?</t>
+  </si>
+  <si>
+    <t>Improvised Weapon Handler</t>
+  </si>
+  <si>
+    <t>Improvsied Weapon Master</t>
+  </si>
+  <si>
+    <t>You gain a +2 bonus to all attack rolls with improvised weapons.</t>
+  </si>
+  <si>
+    <t>Increased Teleportation</t>
+  </si>
+  <si>
+    <t>Capatalize Talent</t>
+  </si>
+  <si>
+    <t>Add the word bonus after +2</t>
+  </si>
+  <si>
+    <t>Lucky Break</t>
+  </si>
+  <si>
+    <t>Natural armor</t>
+  </si>
+  <si>
+    <t>Decapatalize Modifier</t>
+  </si>
+  <si>
+    <t>Power Word II</t>
+  </si>
+  <si>
+    <t>Change to "…whether or not to cast a bound spell…". Alsom capatalize Power Word the second time.</t>
+  </si>
+  <si>
+    <t>Power Word III</t>
+  </si>
+  <si>
+    <t>Capatalize Power Word the second time.</t>
+  </si>
+  <si>
+    <t>Powerful Strike I-V</t>
+  </si>
+  <si>
+    <t>Change to: Increase the damage die for your Melee Weapon from….</t>
+  </si>
+  <si>
+    <t>Practiced Conjurer</t>
+  </si>
+  <si>
+    <t>Capatalize Conjuration</t>
+  </si>
+  <si>
+    <t>Premonition</t>
+  </si>
+  <si>
+    <t>Do we need a comma after or? I'm split</t>
+  </si>
+  <si>
+    <t>CHARACTER SHEET</t>
+  </si>
+  <si>
+    <t>(sorry!!) Decapatalize movement in the Truths.</t>
+  </si>
+  <si>
+    <t>re-aimed strike</t>
+  </si>
+  <si>
+    <t>Is the last comma necessary?</t>
+  </si>
+  <si>
+    <t>Reprogrammable augmentation</t>
+  </si>
+  <si>
+    <t>Change the second paragraph  to: This Talent can be taken multiple times, selecting a different body part each time. If you choose an already augmented body part, you may change the augmentation associated with that body part.</t>
+  </si>
+  <si>
+    <t>Searing Light</t>
+  </si>
+  <si>
+    <t>Undead or unnatural</t>
+  </si>
+  <si>
+    <t>Share the Luck</t>
+  </si>
+  <si>
+    <t>Fortune points is the current stylization</t>
+  </si>
+  <si>
+    <t>Also change a number to any number</t>
+  </si>
+  <si>
+    <t>Skillful archer</t>
+  </si>
+  <si>
+    <t>Capatalize Reflex</t>
+  </si>
+  <si>
+    <t>Really Speedy</t>
+  </si>
+  <si>
+    <t>Decapatalize Move</t>
+  </si>
+  <si>
+    <t>Spt the Opening</t>
+  </si>
+  <si>
+    <t>Change the prereq to Commanding Presence</t>
+  </si>
+  <si>
+    <t>Stunning Critical</t>
+  </si>
+  <si>
+    <t>When you score a critical hit with…</t>
+  </si>
+  <si>
+    <t>Tricky Fighting</t>
+  </si>
+  <si>
+    <t>Provoke opportunity attacks</t>
+  </si>
+  <si>
+    <t>Provokes opportunity attacks.</t>
+  </si>
+  <si>
+    <t>Two weapon critical</t>
+  </si>
+  <si>
+    <t>Off-hand</t>
+  </si>
+  <si>
+    <t>Two weapon fighting</t>
+  </si>
+  <si>
+    <t>Two weapon Striking</t>
+  </si>
+  <si>
+    <t>Two Weapon Mastery</t>
+  </si>
+  <si>
+    <t>If you choose to make multiple melee attacks per rournund, attacks after the first suffer from a cumulative -2 penalty, rather than a -4.
+Change prereqs to a Dex of 60 and Two weapon Fighting</t>
+  </si>
+  <si>
+    <t>You may make multiple melee attacks per turn, one with each weapon you wield, up to your Dexterity Modifier. All attacks after the first have a cumulative -4 penalty. 
+Change prereq to Dex 30.</t>
+  </si>
+  <si>
+    <t>Two weapon Blocking</t>
+  </si>
+  <si>
+    <t>remove prereqs</t>
+  </si>
+  <si>
+    <t>You gain a +1 to attack rolls when you have a weapon in each hand.
+Change prereq to two weapon fighting.</t>
+  </si>
+  <si>
+    <t>Unarmed Accuracy</t>
+  </si>
+  <si>
+    <t>Remove this Talent</t>
+  </si>
+  <si>
+    <t>Versatile Spellcaster</t>
+  </si>
+  <si>
+    <t>Capatalzie Destruction</t>
   </si>
 </sst>
 </file>
@@ -855,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A1:D701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,24 +1313,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1061,10 +1340,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1072,21 +1351,21 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1100,7 +1379,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1111,26 +1390,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1138,26 +1417,23 @@
         <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1165,7 +1441,10 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1173,10 +1452,10 @@
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1184,176 +1463,174 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="300" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="300" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>13</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>13</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>13</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C47" s="2"/>
     </row>
@@ -1362,143 +1639,147 @@
         <v>13</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>14</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>14</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>93</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>16</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1506,21 +1787,21 @@
         <v>16</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>16</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1528,98 +1809,98 @@
         <v>16</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>18</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1627,356 +1908,3023 @@
         <v>18</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C75" s="2"/>
     </row>
     <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>19</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>19</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C80" s="2"/>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>32</v>
+        <v>153</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>20</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C85" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C86" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>32</v>
+      <c r="A87">
+        <v>21</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>152</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>23</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" s="2"/>
+      <c r="A95">
+        <v>24</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>24</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>24</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>25</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>25</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>25</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>25</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>25</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>25</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>25</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>26</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>26</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>26</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>26</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>26</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>26</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>26</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>26</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>27</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>27</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>27</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>27</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>27</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>27</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>28</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>28</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>30</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>60</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>32</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124" s="2"/>
+    <row r="124" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>32</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125" s="2"/>
+    <row r="125" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>32</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="C125" s="2"/>
     </row>
+    <row r="126" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>32</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>32</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C128" s="2"/>
+    </row>
+    <row r="129" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>28</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C130" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>28</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>29</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>29</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>29</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>29</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>28</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>29</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>30</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>30</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>30</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>30</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>30</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>30</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>30</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>30</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>31</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>31</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" s="2"/>
+      <c r="C163" s="2"/>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B169" s="2"/>
+      <c r="C169" s="2"/>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" s="2"/>
+      <c r="C174" s="2"/>
+    </row>
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" s="2"/>
+      <c r="C177" s="2"/>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B181" s="2"/>
+      <c r="C181" s="2"/>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B183" s="2"/>
+      <c r="C183" s="2"/>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B184" s="2"/>
+      <c r="C184" s="2"/>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B188" s="2"/>
+      <c r="C188" s="2"/>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B189" s="2"/>
+      <c r="C189" s="2"/>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B190" s="2"/>
+      <c r="C190" s="2"/>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B191" s="2"/>
+      <c r="C191" s="2"/>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="2"/>
+      <c r="C194" s="2"/>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" s="2"/>
+      <c r="C195" s="2"/>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" s="2"/>
+      <c r="C198" s="2"/>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" s="2"/>
+      <c r="C199" s="2"/>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="2"/>
+      <c r="C200" s="2"/>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" s="2"/>
+      <c r="C201" s="2"/>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B202" s="2"/>
+      <c r="C202" s="2"/>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="2"/>
+      <c r="C203" s="2"/>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="2"/>
+      <c r="C204" s="2"/>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B209" s="2"/>
+      <c r="C209" s="2"/>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="2"/>
+      <c r="C213" s="2"/>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="2"/>
+      <c r="C214" s="2"/>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" s="2"/>
+      <c r="C218" s="2"/>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B221" s="2"/>
+      <c r="C221" s="2"/>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B222" s="2"/>
+      <c r="C222" s="2"/>
+    </row>
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B224" s="2"/>
+      <c r="C224" s="2"/>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B225" s="2"/>
+      <c r="C225" s="2"/>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B226" s="2"/>
+      <c r="C226" s="2"/>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B227" s="2"/>
+      <c r="C227" s="2"/>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B228" s="2"/>
+      <c r="C228" s="2"/>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+    </row>
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B230" s="2"/>
+      <c r="C230" s="2"/>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B231" s="2"/>
+      <c r="C231" s="2"/>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B232" s="2"/>
+      <c r="C232" s="2"/>
+    </row>
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B233" s="2"/>
+      <c r="C233" s="2"/>
+    </row>
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B234" s="2"/>
+      <c r="C234" s="2"/>
+    </row>
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B235" s="2"/>
+      <c r="C235" s="2"/>
+    </row>
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B236" s="2"/>
+      <c r="C236" s="2"/>
+    </row>
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B237" s="2"/>
+      <c r="C237" s="2"/>
+    </row>
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B238" s="2"/>
+      <c r="C238" s="2"/>
+    </row>
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B239" s="2"/>
+      <c r="C239" s="2"/>
+    </row>
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B240" s="2"/>
+      <c r="C240" s="2"/>
+    </row>
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B241" s="2"/>
+      <c r="C241" s="2"/>
+    </row>
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B242" s="2"/>
+      <c r="C242" s="2"/>
+    </row>
+    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B243" s="2"/>
+      <c r="C243" s="2"/>
+    </row>
+    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B244" s="2"/>
+      <c r="C244" s="2"/>
+    </row>
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B245" s="2"/>
+      <c r="C245" s="2"/>
+    </row>
+    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B246" s="2"/>
+      <c r="C246" s="2"/>
+    </row>
+    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B247" s="2"/>
+      <c r="C247" s="2"/>
+    </row>
+    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B248" s="2"/>
+      <c r="C248" s="2"/>
+    </row>
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B249" s="2"/>
+      <c r="C249" s="2"/>
+    </row>
+    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B250" s="2"/>
+      <c r="C250" s="2"/>
+    </row>
+    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B251" s="2"/>
+      <c r="C251" s="2"/>
+    </row>
+    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B252" s="2"/>
+      <c r="C252" s="2"/>
+    </row>
+    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B253" s="2"/>
+      <c r="C253" s="2"/>
+    </row>
+    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B254" s="2"/>
+      <c r="C254" s="2"/>
+    </row>
+    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B255" s="2"/>
+      <c r="C255" s="2"/>
+    </row>
+    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B256" s="2"/>
+      <c r="C256" s="2"/>
+    </row>
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B257" s="2"/>
+      <c r="C257" s="2"/>
+    </row>
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B258" s="2"/>
+      <c r="C258" s="2"/>
+    </row>
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B259" s="2"/>
+      <c r="C259" s="2"/>
+    </row>
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B260" s="2"/>
+      <c r="C260" s="2"/>
+    </row>
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B261" s="2"/>
+      <c r="C261" s="2"/>
+    </row>
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B262" s="2"/>
+      <c r="C262" s="2"/>
+    </row>
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B263" s="2"/>
+      <c r="C263" s="2"/>
+    </row>
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B264" s="2"/>
+      <c r="C264" s="2"/>
+    </row>
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B265" s="2"/>
+      <c r="C265" s="2"/>
+    </row>
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B266" s="2"/>
+      <c r="C266" s="2"/>
+    </row>
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B267" s="2"/>
+      <c r="C267" s="2"/>
+    </row>
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B268" s="2"/>
+      <c r="C268" s="2"/>
+    </row>
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B269" s="2"/>
+      <c r="C269" s="2"/>
+    </row>
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B270" s="2"/>
+      <c r="C270" s="2"/>
+    </row>
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B271" s="2"/>
+      <c r="C271" s="2"/>
+    </row>
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B272" s="2"/>
+      <c r="C272" s="2"/>
+    </row>
+    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B273" s="2"/>
+      <c r="C273" s="2"/>
+    </row>
+    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B274" s="2"/>
+      <c r="C274" s="2"/>
+    </row>
+    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B275" s="2"/>
+      <c r="C275" s="2"/>
+    </row>
+    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B276" s="2"/>
+      <c r="C276" s="2"/>
+    </row>
+    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B277" s="2"/>
+      <c r="C277" s="2"/>
+    </row>
+    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B278" s="2"/>
+      <c r="C278" s="2"/>
+    </row>
+    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B279" s="2"/>
+      <c r="C279" s="2"/>
+    </row>
+    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B280" s="2"/>
+      <c r="C280" s="2"/>
+    </row>
+    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B281" s="2"/>
+      <c r="C281" s="2"/>
+    </row>
+    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B282" s="2"/>
+      <c r="C282" s="2"/>
+    </row>
+    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B283" s="2"/>
+      <c r="C283" s="2"/>
+    </row>
+    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B284" s="2"/>
+      <c r="C284" s="2"/>
+    </row>
+    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B285" s="2"/>
+      <c r="C285" s="2"/>
+    </row>
+    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B286" s="2"/>
+      <c r="C286" s="2"/>
+    </row>
+    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B287" s="2"/>
+      <c r="C287" s="2"/>
+    </row>
+    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B288" s="2"/>
+      <c r="C288" s="2"/>
+    </row>
+    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B289" s="2"/>
+      <c r="C289" s="2"/>
+    </row>
+    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B290" s="2"/>
+      <c r="C290" s="2"/>
+    </row>
+    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B291" s="2"/>
+      <c r="C291" s="2"/>
+    </row>
+    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B292" s="2"/>
+      <c r="C292" s="2"/>
+    </row>
+    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B293" s="2"/>
+      <c r="C293" s="2"/>
+    </row>
+    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B294" s="2"/>
+      <c r="C294" s="2"/>
+    </row>
+    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B295" s="2"/>
+      <c r="C295" s="2"/>
+    </row>
+    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B296" s="2"/>
+      <c r="C296" s="2"/>
+    </row>
+    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B297" s="2"/>
+      <c r="C297" s="2"/>
+    </row>
+    <row r="298" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B298" s="2"/>
+      <c r="C298" s="2"/>
+    </row>
+    <row r="299" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B299" s="2"/>
+      <c r="C299" s="2"/>
+    </row>
+    <row r="300" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B300" s="2"/>
+      <c r="C300" s="2"/>
+    </row>
+    <row r="301" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B301" s="2"/>
+      <c r="C301" s="2"/>
+    </row>
+    <row r="302" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B302" s="2"/>
+      <c r="C302" s="2"/>
+    </row>
+    <row r="303" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B303" s="2"/>
+      <c r="C303" s="2"/>
+    </row>
+    <row r="304" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B304" s="2"/>
+      <c r="C304" s="2"/>
+    </row>
+    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B305" s="2"/>
+      <c r="C305" s="2"/>
+    </row>
+    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B306" s="2"/>
+      <c r="C306" s="2"/>
+    </row>
+    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B307" s="2"/>
+      <c r="C307" s="2"/>
+    </row>
+    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B308" s="2"/>
+      <c r="C308" s="2"/>
+    </row>
+    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B309" s="2"/>
+      <c r="C309" s="2"/>
+    </row>
+    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B310" s="2"/>
+      <c r="C310" s="2"/>
+    </row>
+    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B311" s="2"/>
+      <c r="C311" s="2"/>
+    </row>
+    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B312" s="2"/>
+      <c r="C312" s="2"/>
+    </row>
+    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B313" s="2"/>
+      <c r="C313" s="2"/>
+    </row>
+    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B314" s="2"/>
+      <c r="C314" s="2"/>
+    </row>
+    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B315" s="2"/>
+      <c r="C315" s="2"/>
+    </row>
+    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B316" s="2"/>
+      <c r="C316" s="2"/>
+    </row>
+    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B317" s="2"/>
+      <c r="C317" s="2"/>
+    </row>
+    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B318" s="2"/>
+      <c r="C318" s="2"/>
+    </row>
+    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B319" s="2"/>
+      <c r="C319" s="2"/>
+    </row>
+    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B320" s="2"/>
+      <c r="C320" s="2"/>
+    </row>
+    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B321" s="2"/>
+      <c r="C321" s="2"/>
+    </row>
+    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B322" s="2"/>
+      <c r="C322" s="2"/>
+    </row>
+    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B323" s="2"/>
+      <c r="C323" s="2"/>
+    </row>
+    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B324" s="2"/>
+      <c r="C324" s="2"/>
+    </row>
+    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B325" s="2"/>
+      <c r="C325" s="2"/>
+    </row>
+    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B326" s="2"/>
+      <c r="C326" s="2"/>
+    </row>
+    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B327" s="2"/>
+      <c r="C327" s="2"/>
+    </row>
+    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B328" s="2"/>
+      <c r="C328" s="2"/>
+    </row>
+    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B329" s="2"/>
+      <c r="C329" s="2"/>
+    </row>
+    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B330" s="2"/>
+      <c r="C330" s="2"/>
+    </row>
+    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B331" s="2"/>
+      <c r="C331" s="2"/>
+    </row>
+    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B332" s="2"/>
+      <c r="C332" s="2"/>
+    </row>
+    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B333" s="2"/>
+      <c r="C333" s="2"/>
+    </row>
+    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B334" s="2"/>
+      <c r="C334" s="2"/>
+    </row>
+    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B335" s="2"/>
+      <c r="C335" s="2"/>
+    </row>
+    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B336" s="2"/>
+      <c r="C336" s="2"/>
+    </row>
+    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B337" s="2"/>
+      <c r="C337" s="2"/>
+    </row>
+    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B338" s="2"/>
+      <c r="C338" s="2"/>
+    </row>
+    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B339" s="2"/>
+      <c r="C339" s="2"/>
+    </row>
+    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B340" s="2"/>
+      <c r="C340" s="2"/>
+    </row>
+    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B341" s="2"/>
+      <c r="C341" s="2"/>
+    </row>
+    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B342" s="2"/>
+      <c r="C342" s="2"/>
+    </row>
+    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B343" s="2"/>
+      <c r="C343" s="2"/>
+    </row>
+    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B344" s="2"/>
+      <c r="C344" s="2"/>
+    </row>
+    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B345" s="2"/>
+      <c r="C345" s="2"/>
+    </row>
+    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B346" s="2"/>
+      <c r="C346" s="2"/>
+    </row>
+    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B347" s="2"/>
+      <c r="C347" s="2"/>
+    </row>
+    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B348" s="2"/>
+      <c r="C348" s="2"/>
+    </row>
+    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B349" s="2"/>
+      <c r="C349" s="2"/>
+    </row>
+    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B350" s="2"/>
+      <c r="C350" s="2"/>
+    </row>
+    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B351" s="2"/>
+      <c r="C351" s="2"/>
+    </row>
+    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B352" s="2"/>
+      <c r="C352" s="2"/>
+    </row>
+    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B353" s="2"/>
+      <c r="C353" s="2"/>
+    </row>
+    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B354" s="2"/>
+      <c r="C354" s="2"/>
+    </row>
+    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B355" s="2"/>
+      <c r="C355" s="2"/>
+    </row>
+    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B356" s="2"/>
+      <c r="C356" s="2"/>
+    </row>
+    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B357" s="2"/>
+      <c r="C357" s="2"/>
+    </row>
+    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B358" s="2"/>
+      <c r="C358" s="2"/>
+    </row>
+    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B359" s="2"/>
+      <c r="C359" s="2"/>
+    </row>
+    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B360" s="2"/>
+      <c r="C360" s="2"/>
+    </row>
+    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B361" s="2"/>
+      <c r="C361" s="2"/>
+    </row>
+    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B362" s="2"/>
+      <c r="C362" s="2"/>
+    </row>
+    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B363" s="2"/>
+      <c r="C363" s="2"/>
+    </row>
+    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B364" s="2"/>
+      <c r="C364" s="2"/>
+    </row>
+    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B365" s="2"/>
+      <c r="C365" s="2"/>
+    </row>
+    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B366" s="2"/>
+      <c r="C366" s="2"/>
+    </row>
+    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B367" s="2"/>
+      <c r="C367" s="2"/>
+    </row>
+    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B368" s="2"/>
+      <c r="C368" s="2"/>
+    </row>
+    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B369" s="2"/>
+      <c r="C369" s="2"/>
+    </row>
+    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B370" s="2"/>
+      <c r="C370" s="2"/>
+    </row>
+    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B371" s="2"/>
+      <c r="C371" s="2"/>
+    </row>
+    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B372" s="2"/>
+      <c r="C372" s="2"/>
+    </row>
+    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B373" s="2"/>
+      <c r="C373" s="2"/>
+    </row>
+    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B374" s="2"/>
+      <c r="C374" s="2"/>
+    </row>
+    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B375" s="2"/>
+      <c r="C375" s="2"/>
+    </row>
+    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B376" s="2"/>
+      <c r="C376" s="2"/>
+    </row>
+    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B377" s="2"/>
+      <c r="C377" s="2"/>
+    </row>
+    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B378" s="2"/>
+      <c r="C378" s="2"/>
+    </row>
+    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B379" s="2"/>
+      <c r="C379" s="2"/>
+    </row>
+    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B380" s="2"/>
+      <c r="C380" s="2"/>
+    </row>
+    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B381" s="2"/>
+      <c r="C381" s="2"/>
+    </row>
+    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B382" s="2"/>
+      <c r="C382" s="2"/>
+    </row>
+    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B383" s="2"/>
+      <c r="C383" s="2"/>
+    </row>
+    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B384" s="2"/>
+      <c r="C384" s="2"/>
+    </row>
+    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B385" s="2"/>
+      <c r="C385" s="2"/>
+    </row>
+    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B386" s="2"/>
+      <c r="C386" s="2"/>
+    </row>
+    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B387" s="2"/>
+      <c r="C387" s="2"/>
+    </row>
+    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B388" s="2"/>
+      <c r="C388" s="2"/>
+    </row>
+    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B389" s="2"/>
+      <c r="C389" s="2"/>
+    </row>
+    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B390" s="2"/>
+      <c r="C390" s="2"/>
+    </row>
+    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B391" s="2"/>
+      <c r="C391" s="2"/>
+    </row>
+    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B392" s="2"/>
+      <c r="C392" s="2"/>
+    </row>
+    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B393" s="2"/>
+      <c r="C393" s="2"/>
+    </row>
+    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B394" s="2"/>
+      <c r="C394" s="2"/>
+    </row>
+    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B395" s="2"/>
+      <c r="C395" s="2"/>
+    </row>
+    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B396" s="2"/>
+      <c r="C396" s="2"/>
+    </row>
+    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B397" s="2"/>
+      <c r="C397" s="2"/>
+    </row>
+    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B398" s="2"/>
+      <c r="C398" s="2"/>
+    </row>
+    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B399" s="2"/>
+      <c r="C399" s="2"/>
+    </row>
+    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B400" s="2"/>
+      <c r="C400" s="2"/>
+    </row>
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B401" s="2"/>
+      <c r="C401" s="2"/>
+    </row>
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B402" s="2"/>
+      <c r="C402" s="2"/>
+    </row>
+    <row r="403" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B403" s="2"/>
+      <c r="C403" s="2"/>
+    </row>
+    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B404" s="2"/>
+      <c r="C404" s="2"/>
+    </row>
+    <row r="405" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B405" s="2"/>
+      <c r="C405" s="2"/>
+    </row>
+    <row r="406" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B406" s="2"/>
+      <c r="C406" s="2"/>
+    </row>
+    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B407" s="2"/>
+      <c r="C407" s="2"/>
+    </row>
+    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B408" s="2"/>
+      <c r="C408" s="2"/>
+    </row>
+    <row r="409" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B409" s="2"/>
+      <c r="C409" s="2"/>
+    </row>
+    <row r="410" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B410" s="2"/>
+      <c r="C410" s="2"/>
+    </row>
+    <row r="411" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B411" s="2"/>
+      <c r="C411" s="2"/>
+    </row>
+    <row r="412" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B412" s="2"/>
+      <c r="C412" s="2"/>
+    </row>
+    <row r="413" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B413" s="2"/>
+      <c r="C413" s="2"/>
+    </row>
+    <row r="414" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B414" s="2"/>
+      <c r="C414" s="2"/>
+    </row>
+    <row r="415" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B415" s="2"/>
+      <c r="C415" s="2"/>
+    </row>
+    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B416" s="2"/>
+      <c r="C416" s="2"/>
+    </row>
+    <row r="417" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B417" s="2"/>
+      <c r="C417" s="2"/>
+    </row>
+    <row r="418" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B418" s="2"/>
+      <c r="C418" s="2"/>
+    </row>
+    <row r="419" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B419" s="2"/>
+      <c r="C419" s="2"/>
+    </row>
+    <row r="420" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B420" s="2"/>
+      <c r="C420" s="2"/>
+    </row>
+    <row r="421" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B421" s="2"/>
+      <c r="C421" s="2"/>
+    </row>
+    <row r="422" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B422" s="2"/>
+      <c r="C422" s="2"/>
+    </row>
+    <row r="423" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B423" s="2"/>
+      <c r="C423" s="2"/>
+    </row>
+    <row r="424" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B424" s="2"/>
+      <c r="C424" s="2"/>
+    </row>
+    <row r="425" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B425" s="2"/>
+      <c r="C425" s="2"/>
+    </row>
+    <row r="426" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B426" s="2"/>
+      <c r="C426" s="2"/>
+    </row>
+    <row r="427" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B427" s="2"/>
+      <c r="C427" s="2"/>
+    </row>
+    <row r="428" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B428" s="2"/>
+      <c r="C428" s="2"/>
+    </row>
+    <row r="429" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B429" s="2"/>
+      <c r="C429" s="2"/>
+    </row>
+    <row r="430" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B430" s="2"/>
+      <c r="C430" s="2"/>
+    </row>
+    <row r="431" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B431" s="2"/>
+      <c r="C431" s="2"/>
+    </row>
+    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B432" s="2"/>
+      <c r="C432" s="2"/>
+    </row>
+    <row r="433" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B433" s="2"/>
+      <c r="C433" s="2"/>
+    </row>
+    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B434" s="2"/>
+      <c r="C434" s="2"/>
+    </row>
+    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B435" s="2"/>
+      <c r="C435" s="2"/>
+    </row>
+    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B436" s="2"/>
+      <c r="C436" s="2"/>
+    </row>
+    <row r="437" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B437" s="2"/>
+      <c r="C437" s="2"/>
+    </row>
+    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B438" s="2"/>
+      <c r="C438" s="2"/>
+    </row>
+    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B439" s="2"/>
+      <c r="C439" s="2"/>
+    </row>
+    <row r="440" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B440" s="2"/>
+      <c r="C440" s="2"/>
+    </row>
+    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B441" s="2"/>
+      <c r="C441" s="2"/>
+    </row>
+    <row r="442" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B442" s="2"/>
+      <c r="C442" s="2"/>
+    </row>
+    <row r="443" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B443" s="2"/>
+      <c r="C443" s="2"/>
+    </row>
+    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B444" s="2"/>
+      <c r="C444" s="2"/>
+    </row>
+    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B445" s="2"/>
+      <c r="C445" s="2"/>
+    </row>
+    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B446" s="2"/>
+      <c r="C446" s="2"/>
+    </row>
+    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B447" s="2"/>
+      <c r="C447" s="2"/>
+    </row>
+    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B448" s="2"/>
+      <c r="C448" s="2"/>
+    </row>
+    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B449" s="2"/>
+      <c r="C449" s="2"/>
+    </row>
+    <row r="450" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B450" s="2"/>
+      <c r="C450" s="2"/>
+    </row>
+    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B451" s="2"/>
+      <c r="C451" s="2"/>
+    </row>
+    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B452" s="2"/>
+      <c r="C452" s="2"/>
+    </row>
+    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B453" s="2"/>
+      <c r="C453" s="2"/>
+    </row>
+    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B454" s="2"/>
+      <c r="C454" s="2"/>
+    </row>
+    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B455" s="2"/>
+      <c r="C455" s="2"/>
+    </row>
+    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B456" s="2"/>
+      <c r="C456" s="2"/>
+    </row>
+    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B457" s="2"/>
+      <c r="C457" s="2"/>
+    </row>
+    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B458" s="2"/>
+      <c r="C458" s="2"/>
+    </row>
+    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B459" s="2"/>
+      <c r="C459" s="2"/>
+    </row>
+    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B460" s="2"/>
+      <c r="C460" s="2"/>
+    </row>
+    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B461" s="2"/>
+      <c r="C461" s="2"/>
+    </row>
+    <row r="462" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B462" s="2"/>
+      <c r="C462" s="2"/>
+    </row>
+    <row r="463" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B463" s="2"/>
+      <c r="C463" s="2"/>
+    </row>
+    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B464" s="2"/>
+      <c r="C464" s="2"/>
+    </row>
+    <row r="465" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B465" s="2"/>
+      <c r="C465" s="2"/>
+    </row>
+    <row r="466" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B466" s="2"/>
+      <c r="C466" s="2"/>
+    </row>
+    <row r="467" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B467" s="2"/>
+      <c r="C467" s="2"/>
+    </row>
+    <row r="468" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B468" s="2"/>
+      <c r="C468" s="2"/>
+    </row>
+    <row r="469" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B469" s="2"/>
+      <c r="C469" s="2"/>
+    </row>
+    <row r="470" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B470" s="2"/>
+      <c r="C470" s="2"/>
+    </row>
+    <row r="471" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B471" s="2"/>
+      <c r="C471" s="2"/>
+    </row>
+    <row r="472" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B472" s="2"/>
+      <c r="C472" s="2"/>
+    </row>
+    <row r="473" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B473" s="2"/>
+      <c r="C473" s="2"/>
+    </row>
+    <row r="474" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B474" s="2"/>
+      <c r="C474" s="2"/>
+    </row>
+    <row r="475" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B475" s="2"/>
+      <c r="C475" s="2"/>
+    </row>
+    <row r="476" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B476" s="2"/>
+      <c r="C476" s="2"/>
+    </row>
+    <row r="477" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B477" s="2"/>
+      <c r="C477" s="2"/>
+    </row>
+    <row r="478" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B478" s="2"/>
+      <c r="C478" s="2"/>
+    </row>
+    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B479" s="2"/>
+      <c r="C479" s="2"/>
+    </row>
+    <row r="480" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B480" s="2"/>
+      <c r="C480" s="2"/>
+    </row>
+    <row r="481" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B481" s="2"/>
+      <c r="C481" s="2"/>
+    </row>
+    <row r="482" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B482" s="2"/>
+      <c r="C482" s="2"/>
+    </row>
+    <row r="483" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B483" s="2"/>
+      <c r="C483" s="2"/>
+    </row>
+    <row r="484" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B484" s="2"/>
+      <c r="C484" s="2"/>
+    </row>
+    <row r="485" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B485" s="2"/>
+      <c r="C485" s="2"/>
+    </row>
+    <row r="486" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B486" s="2"/>
+      <c r="C486" s="2"/>
+    </row>
+    <row r="487" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B487" s="2"/>
+      <c r="C487" s="2"/>
+    </row>
+    <row r="488" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B488" s="2"/>
+      <c r="C488" s="2"/>
+    </row>
+    <row r="489" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B489" s="2"/>
+      <c r="C489" s="2"/>
+    </row>
+    <row r="490" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B490" s="2"/>
+      <c r="C490" s="2"/>
+    </row>
+    <row r="491" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B491" s="2"/>
+      <c r="C491" s="2"/>
+    </row>
+    <row r="492" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B492" s="2"/>
+      <c r="C492" s="2"/>
+    </row>
+    <row r="493" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B493" s="2"/>
+      <c r="C493" s="2"/>
+    </row>
+    <row r="494" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B494" s="2"/>
+      <c r="C494" s="2"/>
+    </row>
+    <row r="495" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B495" s="2"/>
+      <c r="C495" s="2"/>
+    </row>
+    <row r="496" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B496" s="2"/>
+      <c r="C496" s="2"/>
+    </row>
+    <row r="497" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B497" s="2"/>
+      <c r="C497" s="2"/>
+    </row>
+    <row r="498" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B498" s="2"/>
+      <c r="C498" s="2"/>
+    </row>
+    <row r="499" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B499" s="2"/>
+      <c r="C499" s="2"/>
+    </row>
+    <row r="500" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B500" s="2"/>
+      <c r="C500" s="2"/>
+    </row>
+    <row r="501" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B501" s="2"/>
+      <c r="C501" s="2"/>
+    </row>
+    <row r="502" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B502" s="2"/>
+      <c r="C502" s="2"/>
+    </row>
+    <row r="503" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B503" s="2"/>
+      <c r="C503" s="2"/>
+    </row>
+    <row r="504" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B504" s="2"/>
+      <c r="C504" s="2"/>
+    </row>
+    <row r="505" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B505" s="2"/>
+      <c r="C505" s="2"/>
+    </row>
+    <row r="506" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B506" s="2"/>
+      <c r="C506" s="2"/>
+    </row>
+    <row r="507" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B507" s="2"/>
+      <c r="C507" s="2"/>
+    </row>
+    <row r="508" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B508" s="2"/>
+      <c r="C508" s="2"/>
+    </row>
+    <row r="509" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B509" s="2"/>
+      <c r="C509" s="2"/>
+    </row>
+    <row r="510" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B510" s="2"/>
+      <c r="C510" s="2"/>
+    </row>
+    <row r="511" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B511" s="2"/>
+      <c r="C511" s="2"/>
+    </row>
+    <row r="512" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B512" s="2"/>
+      <c r="C512" s="2"/>
+    </row>
+    <row r="513" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B513" s="2"/>
+      <c r="C513" s="2"/>
+    </row>
+    <row r="514" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B514" s="2"/>
+      <c r="C514" s="2"/>
+    </row>
+    <row r="515" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B515" s="2"/>
+      <c r="C515" s="2"/>
+    </row>
+    <row r="516" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B516" s="2"/>
+      <c r="C516" s="2"/>
+    </row>
+    <row r="517" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B517" s="2"/>
+      <c r="C517" s="2"/>
+    </row>
+    <row r="518" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B518" s="2"/>
+      <c r="C518" s="2"/>
+    </row>
+    <row r="519" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B519" s="2"/>
+      <c r="C519" s="2"/>
+    </row>
+    <row r="520" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B520" s="2"/>
+      <c r="C520" s="2"/>
+    </row>
+    <row r="521" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B521" s="2"/>
+      <c r="C521" s="2"/>
+    </row>
+    <row r="522" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B522" s="2"/>
+      <c r="C522" s="2"/>
+    </row>
+    <row r="523" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B523" s="2"/>
+      <c r="C523" s="2"/>
+    </row>
+    <row r="524" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B524" s="2"/>
+      <c r="C524" s="2"/>
+    </row>
+    <row r="525" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B525" s="2"/>
+      <c r="C525" s="2"/>
+    </row>
+    <row r="526" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B526" s="2"/>
+      <c r="C526" s="2"/>
+    </row>
+    <row r="527" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B527" s="2"/>
+      <c r="C527" s="2"/>
+    </row>
+    <row r="528" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B528" s="2"/>
+      <c r="C528" s="2"/>
+    </row>
+    <row r="529" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B529" s="2"/>
+      <c r="C529" s="2"/>
+    </row>
+    <row r="530" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B530" s="2"/>
+      <c r="C530" s="2"/>
+    </row>
+    <row r="531" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B531" s="2"/>
+      <c r="C531" s="2"/>
+    </row>
+    <row r="532" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B532" s="2"/>
+      <c r="C532" s="2"/>
+    </row>
+    <row r="533" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B533" s="2"/>
+      <c r="C533" s="2"/>
+    </row>
+    <row r="534" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B534" s="2"/>
+      <c r="C534" s="2"/>
+    </row>
+    <row r="535" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B535" s="2"/>
+      <c r="C535" s="2"/>
+    </row>
+    <row r="536" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B536" s="2"/>
+      <c r="C536" s="2"/>
+    </row>
+    <row r="537" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B537" s="2"/>
+      <c r="C537" s="2"/>
+    </row>
+    <row r="538" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B538" s="2"/>
+      <c r="C538" s="2"/>
+    </row>
+    <row r="539" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B539" s="2"/>
+      <c r="C539" s="2"/>
+    </row>
+    <row r="540" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B540" s="2"/>
+      <c r="C540" s="2"/>
+    </row>
+    <row r="541" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B541" s="2"/>
+      <c r="C541" s="2"/>
+    </row>
+    <row r="542" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B542" s="2"/>
+      <c r="C542" s="2"/>
+    </row>
+    <row r="543" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B543" s="2"/>
+      <c r="C543" s="2"/>
+    </row>
+    <row r="544" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B544" s="2"/>
+      <c r="C544" s="2"/>
+    </row>
+    <row r="545" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B545" s="2"/>
+      <c r="C545" s="2"/>
+    </row>
+    <row r="546" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B546" s="2"/>
+      <c r="C546" s="2"/>
+    </row>
+    <row r="547" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B547" s="2"/>
+      <c r="C547" s="2"/>
+    </row>
+    <row r="548" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B548" s="2"/>
+      <c r="C548" s="2"/>
+    </row>
+    <row r="549" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B549" s="2"/>
+      <c r="C549" s="2"/>
+    </row>
+    <row r="550" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B550" s="2"/>
+      <c r="C550" s="2"/>
+    </row>
+    <row r="551" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B551" s="2"/>
+      <c r="C551" s="2"/>
+    </row>
+    <row r="552" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B552" s="2"/>
+      <c r="C552" s="2"/>
+    </row>
+    <row r="553" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B553" s="2"/>
+      <c r="C553" s="2"/>
+    </row>
+    <row r="554" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B554" s="2"/>
+      <c r="C554" s="2"/>
+    </row>
+    <row r="555" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B555" s="2"/>
+      <c r="C555" s="2"/>
+    </row>
+    <row r="556" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B556" s="2"/>
+      <c r="C556" s="2"/>
+    </row>
+    <row r="557" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B557" s="2"/>
+      <c r="C557" s="2"/>
+    </row>
+    <row r="558" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B558" s="2"/>
+      <c r="C558" s="2"/>
+    </row>
+    <row r="559" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B559" s="2"/>
+      <c r="C559" s="2"/>
+    </row>
+    <row r="560" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B560" s="2"/>
+      <c r="C560" s="2"/>
+    </row>
+    <row r="561" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B561" s="2"/>
+      <c r="C561" s="2"/>
+    </row>
+    <row r="562" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B562" s="2"/>
+      <c r="C562" s="2"/>
+    </row>
+    <row r="563" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B563" s="2"/>
+      <c r="C563" s="2"/>
+    </row>
+    <row r="564" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B564" s="2"/>
+      <c r="C564" s="2"/>
+    </row>
+    <row r="565" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B565" s="2"/>
+      <c r="C565" s="2"/>
+    </row>
+    <row r="566" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B566" s="2"/>
+      <c r="C566" s="2"/>
+    </row>
+    <row r="567" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B567" s="2"/>
+      <c r="C567" s="2"/>
+    </row>
+    <row r="568" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B568" s="2"/>
+      <c r="C568" s="2"/>
+    </row>
+    <row r="569" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B569" s="2"/>
+      <c r="C569" s="2"/>
+    </row>
+    <row r="570" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B570" s="2"/>
+      <c r="C570" s="2"/>
+    </row>
+    <row r="571" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B571" s="2"/>
+      <c r="C571" s="2"/>
+    </row>
+    <row r="572" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B572" s="2"/>
+      <c r="C572" s="2"/>
+    </row>
+    <row r="573" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B573" s="2"/>
+      <c r="C573" s="2"/>
+    </row>
+    <row r="574" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B574" s="2"/>
+      <c r="C574" s="2"/>
+    </row>
+    <row r="575" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B575" s="2"/>
+      <c r="C575" s="2"/>
+    </row>
+    <row r="576" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B576" s="2"/>
+      <c r="C576" s="2"/>
+    </row>
+    <row r="577" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B577" s="2"/>
+      <c r="C577" s="2"/>
+    </row>
+    <row r="578" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B578" s="2"/>
+      <c r="C578" s="2"/>
+    </row>
+    <row r="579" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B579" s="2"/>
+      <c r="C579" s="2"/>
+    </row>
+    <row r="580" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B580" s="2"/>
+      <c r="C580" s="2"/>
+    </row>
+    <row r="581" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B581" s="2"/>
+      <c r="C581" s="2"/>
+    </row>
+    <row r="582" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B582" s="2"/>
+      <c r="C582" s="2"/>
+    </row>
+    <row r="583" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B583" s="2"/>
+      <c r="C583" s="2"/>
+    </row>
+    <row r="584" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B584" s="2"/>
+      <c r="C584" s="2"/>
+    </row>
+    <row r="585" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B585" s="2"/>
+      <c r="C585" s="2"/>
+    </row>
+    <row r="586" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B586" s="2"/>
+      <c r="C586" s="2"/>
+    </row>
+    <row r="587" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B587" s="2"/>
+      <c r="C587" s="2"/>
+    </row>
+    <row r="588" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B588" s="2"/>
+      <c r="C588" s="2"/>
+    </row>
+    <row r="589" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B589" s="2"/>
+      <c r="C589" s="2"/>
+    </row>
+    <row r="590" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B590" s="2"/>
+      <c r="C590" s="2"/>
+    </row>
+    <row r="591" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B591" s="2"/>
+      <c r="C591" s="2"/>
+    </row>
+    <row r="592" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B592" s="2"/>
+      <c r="C592" s="2"/>
+    </row>
+    <row r="593" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B593" s="2"/>
+      <c r="C593" s="2"/>
+    </row>
+    <row r="594" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B594" s="2"/>
+      <c r="C594" s="2"/>
+    </row>
+    <row r="595" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B595" s="2"/>
+      <c r="C595" s="2"/>
+    </row>
+    <row r="596" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B596" s="2"/>
+      <c r="C596" s="2"/>
+    </row>
+    <row r="597" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B597" s="2"/>
+      <c r="C597" s="2"/>
+    </row>
+    <row r="598" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B598" s="2"/>
+      <c r="C598" s="2"/>
+    </row>
+    <row r="599" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B599" s="2"/>
+      <c r="C599" s="2"/>
+    </row>
+    <row r="600" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B600" s="2"/>
+      <c r="C600" s="2"/>
+    </row>
+    <row r="601" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B601" s="2"/>
+      <c r="C601" s="2"/>
+    </row>
+    <row r="602" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B602" s="2"/>
+      <c r="C602" s="2"/>
+    </row>
+    <row r="603" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B603" s="2"/>
+      <c r="C603" s="2"/>
+    </row>
+    <row r="604" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B604" s="2"/>
+      <c r="C604" s="2"/>
+    </row>
+    <row r="605" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B605" s="2"/>
+      <c r="C605" s="2"/>
+    </row>
+    <row r="606" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B606" s="2"/>
+      <c r="C606" s="2"/>
+    </row>
+    <row r="607" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B607" s="2"/>
+      <c r="C607" s="2"/>
+    </row>
+    <row r="608" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B608" s="2"/>
+      <c r="C608" s="2"/>
+    </row>
+    <row r="609" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B609" s="2"/>
+      <c r="C609" s="2"/>
+    </row>
+    <row r="610" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B610" s="2"/>
+      <c r="C610" s="2"/>
+    </row>
+    <row r="611" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B611" s="2"/>
+      <c r="C611" s="2"/>
+    </row>
+    <row r="612" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B612" s="2"/>
+      <c r="C612" s="2"/>
+    </row>
+    <row r="613" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B613" s="2"/>
+      <c r="C613" s="2"/>
+    </row>
+    <row r="614" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B614" s="2"/>
+      <c r="C614" s="2"/>
+    </row>
+    <row r="615" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B615" s="2"/>
+      <c r="C615" s="2"/>
+    </row>
+    <row r="616" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B616" s="2"/>
+      <c r="C616" s="2"/>
+    </row>
+    <row r="617" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B617" s="2"/>
+      <c r="C617" s="2"/>
+    </row>
+    <row r="618" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B618" s="2"/>
+      <c r="C618" s="2"/>
+    </row>
+    <row r="619" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B619" s="2"/>
+      <c r="C619" s="2"/>
+    </row>
+    <row r="620" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B620" s="2"/>
+      <c r="C620" s="2"/>
+    </row>
+    <row r="621" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B621" s="2"/>
+      <c r="C621" s="2"/>
+    </row>
+    <row r="622" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B622" s="2"/>
+      <c r="C622" s="2"/>
+    </row>
+    <row r="623" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B623" s="2"/>
+      <c r="C623" s="2"/>
+    </row>
+    <row r="624" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B624" s="2"/>
+      <c r="C624" s="2"/>
+    </row>
+    <row r="625" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B625" s="2"/>
+      <c r="C625" s="2"/>
+    </row>
+    <row r="626" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B626" s="2"/>
+      <c r="C626" s="2"/>
+    </row>
+    <row r="627" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B627" s="2"/>
+      <c r="C627" s="2"/>
+    </row>
+    <row r="628" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B628" s="2"/>
+      <c r="C628" s="2"/>
+    </row>
+    <row r="629" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B629" s="2"/>
+      <c r="C629" s="2"/>
+    </row>
+    <row r="630" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B630" s="2"/>
+      <c r="C630" s="2"/>
+    </row>
+    <row r="631" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B631" s="2"/>
+      <c r="C631" s="2"/>
+    </row>
+    <row r="632" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B632" s="2"/>
+      <c r="C632" s="2"/>
+    </row>
+    <row r="633" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B633" s="2"/>
+      <c r="C633" s="2"/>
+    </row>
+    <row r="634" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B634" s="2"/>
+      <c r="C634" s="2"/>
+    </row>
+    <row r="635" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B635" s="2"/>
+      <c r="C635" s="2"/>
+    </row>
+    <row r="636" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B636" s="2"/>
+      <c r="C636" s="2"/>
+    </row>
+    <row r="637" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B637" s="2"/>
+      <c r="C637" s="2"/>
+    </row>
+    <row r="638" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B638" s="2"/>
+      <c r="C638" s="2"/>
+    </row>
+    <row r="639" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B639" s="2"/>
+      <c r="C639" s="2"/>
+    </row>
+    <row r="640" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B640" s="2"/>
+      <c r="C640" s="2"/>
+    </row>
+    <row r="641" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B641" s="2"/>
+      <c r="C641" s="2"/>
+    </row>
+    <row r="642" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B642" s="2"/>
+      <c r="C642" s="2"/>
+    </row>
+    <row r="643" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B643" s="2"/>
+      <c r="C643" s="2"/>
+    </row>
+    <row r="644" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B644" s="2"/>
+      <c r="C644" s="2"/>
+    </row>
+    <row r="645" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B645" s="2"/>
+      <c r="C645" s="2"/>
+    </row>
+    <row r="646" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B646" s="2"/>
+      <c r="C646" s="2"/>
+    </row>
+    <row r="647" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B647" s="2"/>
+      <c r="C647" s="2"/>
+    </row>
+    <row r="648" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B648" s="2"/>
+      <c r="C648" s="2"/>
+    </row>
+    <row r="649" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B649" s="2"/>
+      <c r="C649" s="2"/>
+    </row>
+    <row r="650" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B650" s="2"/>
+      <c r="C650" s="2"/>
+    </row>
+    <row r="651" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B651" s="2"/>
+      <c r="C651" s="2"/>
+    </row>
+    <row r="652" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B652" s="2"/>
+      <c r="C652" s="2"/>
+    </row>
+    <row r="653" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B653" s="2"/>
+      <c r="C653" s="2"/>
+    </row>
+    <row r="654" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B654" s="2"/>
+      <c r="C654" s="2"/>
+    </row>
+    <row r="655" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B655" s="2"/>
+      <c r="C655" s="2"/>
+    </row>
+    <row r="656" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B656" s="2"/>
+      <c r="C656" s="2"/>
+    </row>
+    <row r="657" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B657" s="2"/>
+      <c r="C657" s="2"/>
+    </row>
+    <row r="658" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B658" s="2"/>
+      <c r="C658" s="2"/>
+    </row>
+    <row r="659" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B659" s="2"/>
+      <c r="C659" s="2"/>
+    </row>
+    <row r="660" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B660" s="2"/>
+      <c r="C660" s="2"/>
+    </row>
+    <row r="661" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B661" s="2"/>
+      <c r="C661" s="2"/>
+    </row>
+    <row r="662" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B662" s="2"/>
+      <c r="C662" s="2"/>
+    </row>
+    <row r="663" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B663" s="2"/>
+      <c r="C663" s="2"/>
+    </row>
+    <row r="664" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B664" s="2"/>
+      <c r="C664" s="2"/>
+    </row>
+    <row r="665" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B665" s="2"/>
+      <c r="C665" s="2"/>
+    </row>
+    <row r="666" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B666" s="2"/>
+      <c r="C666" s="2"/>
+    </row>
+    <row r="667" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B667" s="2"/>
+      <c r="C667" s="2"/>
+    </row>
+    <row r="668" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B668" s="2"/>
+      <c r="C668" s="2"/>
+    </row>
+    <row r="669" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B669" s="2"/>
+      <c r="C669" s="2"/>
+    </row>
+    <row r="670" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B670" s="2"/>
+      <c r="C670" s="2"/>
+    </row>
+    <row r="671" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B671" s="2"/>
+      <c r="C671" s="2"/>
+    </row>
+    <row r="672" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B672" s="2"/>
+      <c r="C672" s="2"/>
+    </row>
+    <row r="673" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B673" s="2"/>
+      <c r="C673" s="2"/>
+    </row>
+    <row r="674" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B674" s="2"/>
+      <c r="C674" s="2"/>
+    </row>
+    <row r="675" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B675" s="2"/>
+      <c r="C675" s="2"/>
+    </row>
+    <row r="676" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B676" s="2"/>
+      <c r="C676" s="2"/>
+    </row>
+    <row r="677" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B677" s="2"/>
+      <c r="C677" s="2"/>
+    </row>
+    <row r="678" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B678" s="2"/>
+      <c r="C678" s="2"/>
+    </row>
+    <row r="679" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B679" s="2"/>
+      <c r="C679" s="2"/>
+    </row>
+    <row r="680" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B680" s="2"/>
+      <c r="C680" s="2"/>
+    </row>
+    <row r="681" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B681" s="2"/>
+      <c r="C681" s="2"/>
+    </row>
+    <row r="682" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B682" s="2"/>
+      <c r="C682" s="2"/>
+    </row>
+    <row r="683" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B683" s="2"/>
+      <c r="C683" s="2"/>
+    </row>
+    <row r="684" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B684" s="2"/>
+      <c r="C684" s="2"/>
+    </row>
+    <row r="685" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B685" s="2"/>
+      <c r="C685" s="2"/>
+    </row>
+    <row r="686" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B686" s="2"/>
+      <c r="C686" s="2"/>
+    </row>
+    <row r="687" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B687" s="2"/>
+      <c r="C687" s="2"/>
+    </row>
+    <row r="688" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B688" s="2"/>
+      <c r="C688" s="2"/>
+    </row>
+    <row r="689" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B689" s="2"/>
+      <c r="C689" s="2"/>
+    </row>
+    <row r="690" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B690" s="2"/>
+      <c r="C690" s="2"/>
+    </row>
+    <row r="691" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B691" s="2"/>
+      <c r="C691" s="2"/>
+    </row>
+    <row r="692" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B692" s="2"/>
+      <c r="C692" s="2"/>
+    </row>
+    <row r="693" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B693" s="2"/>
+      <c r="C693" s="2"/>
+    </row>
+    <row r="694" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B694" s="2"/>
+      <c r="C694" s="2"/>
+    </row>
+    <row r="695" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B695" s="2"/>
+      <c r="C695" s="2"/>
+    </row>
+    <row r="696" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B696" s="2"/>
+      <c r="C696" s="2"/>
+    </row>
+    <row r="697" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B697" s="2"/>
+      <c r="C697" s="2"/>
+    </row>
+    <row r="698" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B698" s="2"/>
+      <c r="C698" s="2"/>
+    </row>
+    <row r="699" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B699" s="2"/>
+      <c r="C699" s="2"/>
+    </row>
+    <row r="700" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B700" s="2"/>
+      <c r="C700" s="2"/>
+    </row>
+    <row r="701" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B701" s="2"/>
+      <c r="C701" s="2"/>
+    </row>
   </sheetData>
+  <sortState ref="A2:D128">
+    <sortCondition ref="A112"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added logo to repo, closed all skill-related issues (renamed nature, moved light armor, security, nature/survival, renamed craft/smith, removed discipline, removed endurance. Began proofreading updates.
</commit_message>
<xml_diff>
--- a/TODO/Proofreading.xlsx
+++ b/TODO/Proofreading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="532">
   <si>
     <t>Page</t>
   </si>
@@ -1986,16 +1986,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E727"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="A320" sqref="A320"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2123,6 +2124,9 @@
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E9" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2134,6 +2138,9 @@
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E10" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2145,6 +2152,9 @@
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E11" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2156,6 +2166,9 @@
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E12" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2167,6 +2180,9 @@
       <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E13" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2178,6 +2194,9 @@
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="E14" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2189,6 +2208,9 @@
       <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="E15" s="6" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -2200,8 +2222,11 @@
       <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2212,7 +2237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2223,7 +2248,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2234,7 +2259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2244,8 +2269,11 @@
       <c r="C20" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2256,7 +2284,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2267,7 +2295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -2278,7 +2306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2289,7 +2317,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2297,7 +2325,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2305,7 +2333,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2313,7 +2341,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -2324,7 +2352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -2335,7 +2363,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9</v>
       </c>
@@ -2344,7 +2372,7 @@
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
@@ -2353,7 +2381,7 @@
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Closed a couple hundred issues. Opened less than 12.
</commit_message>
<xml_diff>
--- a/TODO/Proofreading.xlsx
+++ b/TODO/Proofreading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="539">
   <si>
     <t>Page</t>
   </si>
@@ -1333,12 +1333,6 @@
     <t>opp attacks</t>
   </si>
   <si>
-    <t>can we bold NOT</t>
-  </si>
-  <si>
-    <t>throwing a creature or object</t>
-  </si>
-  <si>
     <t>glass modifier</t>
   </si>
   <si>
@@ -1369,9 +1363,6 @@
     <t>dying</t>
   </si>
   <si>
-    <t>see: death, dying, and the unconscious condition</t>
-  </si>
-  <si>
     <t>63/65</t>
   </si>
   <si>
@@ -1406,12 +1397,6 @@
   </si>
   <si>
     <t>Death, dying, unconscious</t>
-  </si>
-  <si>
-    <t>Extra space before paragraph?</t>
-  </si>
-  <si>
-    <t>Maybe the first sentence should be removed?</t>
   </si>
   <si>
     <t>….they will immediately die.A</t>
@@ -1608,6 +1593,54 @@
   </si>
   <si>
     <t>Restoration range and the like is stylized like this: lowercase range.</t>
+  </si>
+  <si>
+    <t>We appear to have lost a lot of text and a table on page 60. If you need to see what it should look like, ask me or check the docm.</t>
+  </si>
+  <si>
+    <t>:(</t>
+  </si>
+  <si>
+    <t>General note to Rachel</t>
+  </si>
+  <si>
+    <t>I removed penalties to attacking with an off-hand weapon. You can hold two weapons and attack with either one equally well, we say.  Also I defined "off-hand weapon" as any weapon you attack with after your first attack. This makes dual wielding easier later on.</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>No action needed</t>
+  </si>
+  <si>
+    <t>can we bold NOT, or otherwise emphasis this change in lists?</t>
+  </si>
+  <si>
+    <t>throwing a creature or object (uhh when does this become a ranged attack? Maybe need to re-evaluate)</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>see: death, dying, and the unconscious condition, add a reference</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>I'm not sure what this is referring to. Feel free to ignore</t>
+  </si>
+  <si>
+    <t>Extra space before paragraph? Is this intentional?</t>
+  </si>
+  <si>
+    <t>Maybe the first sentence should be removed? Up to you, Rachel</t>
+  </si>
+  <si>
+    <t>I removed it from combat section, but…do we even particularly need this effect?</t>
+  </si>
+  <si>
+    <t>We break our alphabetization here, and then repeat some things. I don't care how, but we should clean this up</t>
   </si>
 </sst>
 </file>
@@ -1975,8 +2008,8 @@
   <dimension ref="A1:E721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E310" sqref="E310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,6 +2018,7 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,7 +2035,7 @@
         <v>23</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2015,7 +2049,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2029,7 +2063,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2043,7 +2077,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2057,7 +2091,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2071,7 +2105,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2085,7 +2119,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2099,7 +2133,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2113,7 +2147,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2127,7 +2161,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2141,7 +2175,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2155,7 +2189,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2169,7 +2203,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2183,7 +2217,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2197,7 +2231,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2211,7 +2245,7 @@
         <v>34</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2258,7 +2292,7 @@
         <v>179</v>
       </c>
       <c r="E20" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2305,7 +2339,7 @@
         <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2316,7 +2350,7 @@
         <v>51</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2327,7 +2361,7 @@
         <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2338,7 +2372,7 @@
         <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2352,7 +2386,7 @@
         <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2366,7 +2400,7 @@
         <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2378,7 +2412,7 @@
       </c>
       <c r="C30" s="2"/>
       <c r="E30" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2390,7 +2424,7 @@
       </c>
       <c r="C31" s="2"/>
       <c r="E31" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2404,7 +2438,7 @@
         <v>61</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2418,7 +2452,7 @@
         <v>65</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="300" x14ac:dyDescent="0.25">
@@ -2432,7 +2466,7 @@
         <v>67</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2444,7 +2478,7 @@
       </c>
       <c r="C35" s="2"/>
       <c r="E35" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2458,7 +2492,7 @@
         <v>70</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2472,7 +2506,7 @@
         <v>74</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2484,7 +2518,7 @@
       </c>
       <c r="C38" s="2"/>
       <c r="E38" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2496,7 +2530,7 @@
       </c>
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2510,7 +2544,7 @@
         <v>93</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2524,7 +2558,7 @@
         <v>95</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2536,7 +2570,7 @@
       </c>
       <c r="C42" s="2"/>
       <c r="E42" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2548,7 +2582,7 @@
       </c>
       <c r="C43" s="2"/>
       <c r="E43" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2560,7 +2594,7 @@
       </c>
       <c r="C44" s="2"/>
       <c r="E44" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="180" x14ac:dyDescent="0.25">
@@ -2572,7 +2606,7 @@
       </c>
       <c r="C45" s="2"/>
       <c r="E45" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2584,7 +2618,7 @@
       </c>
       <c r="C46" s="2"/>
       <c r="E46" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2596,7 +2630,7 @@
       </c>
       <c r="C47" s="2"/>
       <c r="E47" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2608,7 +2642,7 @@
       </c>
       <c r="C48" s="2"/>
       <c r="E48" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2622,7 +2656,7 @@
         <v>85</v>
       </c>
       <c r="E49" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2636,7 +2670,7 @@
         <v>87</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2650,7 +2684,7 @@
         <v>89</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2664,7 +2698,7 @@
         <v>91</v>
       </c>
       <c r="E52" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2676,7 +2710,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="E53" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2688,7 +2722,7 @@
       </c>
       <c r="C54" s="2"/>
       <c r="E54" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2702,7 +2736,7 @@
         <v>99</v>
       </c>
       <c r="E55" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2716,7 +2750,7 @@
         <v>99</v>
       </c>
       <c r="E56" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2730,7 +2764,7 @@
         <v>99</v>
       </c>
       <c r="E57" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2744,7 +2778,7 @@
         <v>103</v>
       </c>
       <c r="E58" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2758,7 +2792,7 @@
         <v>105</v>
       </c>
       <c r="E59" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2772,7 +2806,7 @@
         <v>107</v>
       </c>
       <c r="E60" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2786,7 +2820,7 @@
         <v>109</v>
       </c>
       <c r="E61" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2800,7 +2834,7 @@
         <v>111</v>
       </c>
       <c r="E62" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2814,7 +2848,7 @@
         <v>113</v>
       </c>
       <c r="E63" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2828,7 +2862,7 @@
         <v>115</v>
       </c>
       <c r="E64" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2842,7 +2876,7 @@
         <v>117</v>
       </c>
       <c r="E65" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2856,7 +2890,7 @@
         <v>119</v>
       </c>
       <c r="E66" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2870,7 +2904,7 @@
         <v>120</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2884,7 +2918,7 @@
         <v>122</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2898,7 +2932,7 @@
         <v>124</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2912,7 +2946,7 @@
         <v>126</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2926,7 +2960,7 @@
         <v>127</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2940,7 +2974,7 @@
         <v>129</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2954,7 +2988,7 @@
         <v>131</v>
       </c>
       <c r="E73" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2968,7 +3002,7 @@
         <v>133</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2980,7 +3014,7 @@
       </c>
       <c r="C75" s="2"/>
       <c r="E75" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2994,7 +3028,7 @@
         <v>136</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3008,7 +3042,7 @@
         <v>138</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3022,7 +3056,7 @@
         <v>140</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3036,7 +3070,7 @@
         <v>142</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3048,7 +3082,7 @@
       </c>
       <c r="C80" s="2"/>
       <c r="E80" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3060,7 +3094,7 @@
       </c>
       <c r="C81" s="2"/>
       <c r="E81" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3074,7 +3108,7 @@
         <v>146</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3088,7 +3122,7 @@
         <v>148</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3102,7 +3136,7 @@
         <v>150</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3116,7 +3150,7 @@
         <v>152</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3130,7 +3164,7 @@
         <v>63</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3144,7 +3178,7 @@
         <v>154</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3158,7 +3192,7 @@
         <v>157</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3170,7 +3204,7 @@
       </c>
       <c r="C89" s="2"/>
       <c r="E89" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3184,7 +3218,7 @@
         <v>159</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3198,7 +3232,7 @@
         <v>161</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3221,7 +3255,7 @@
         <v>164</v>
       </c>
       <c r="E93" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3235,7 +3269,7 @@
         <v>189</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3249,7 +3283,7 @@
         <v>166</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3263,7 +3297,7 @@
         <v>168</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3277,7 +3311,7 @@
         <v>175</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3303,7 +3337,7 @@
         <v>177</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3317,7 +3351,7 @@
         <v>170</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -3325,13 +3359,13 @@
         <v>25</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3345,7 +3379,7 @@
         <v>183</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,7 +3393,7 @@
         <v>186</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3373,7 +3407,7 @@
         <v>188</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3387,7 +3421,7 @@
         <v>170</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3401,7 +3435,7 @@
         <v>189</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3415,7 +3449,7 @@
         <v>183</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3429,7 +3463,7 @@
         <v>192</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3443,7 +3477,7 @@
         <v>194</v>
       </c>
       <c r="E109" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3457,7 +3491,7 @@
         <v>195</v>
       </c>
       <c r="E110" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3471,7 +3505,7 @@
         <v>194</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3485,7 +3519,7 @@
         <v>198</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3499,10 +3533,10 @@
         <v>170</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>27</v>
       </c>
@@ -3513,7 +3547,7 @@
         <v>200</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3527,7 +3561,7 @@
         <v>202</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3541,7 +3575,7 @@
         <v>204</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,7 +3589,7 @@
         <v>206</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3569,7 +3603,7 @@
         <v>208</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,7 +3617,7 @@
         <v>170</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,7 +3631,7 @@
         <v>170</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3611,7 +3645,7 @@
         <v>170</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3625,7 +3659,7 @@
         <v>72</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3647,7 +3681,7 @@
         <v>212</v>
       </c>
       <c r="E124" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -3661,7 +3695,7 @@
         <v>214</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3675,7 +3709,7 @@
         <v>216</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3689,7 +3723,7 @@
         <v>218</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3703,7 +3737,7 @@
         <v>219</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3717,7 +3751,7 @@
         <v>221</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3731,7 +3765,7 @@
         <v>223</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3745,7 +3779,7 @@
         <v>225</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3759,7 +3793,7 @@
         <v>227</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3773,7 +3807,7 @@
         <v>229</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3787,7 +3821,7 @@
         <v>230</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3801,7 +3835,7 @@
         <v>232</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -3826,7 +3860,7 @@
         <v>240</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="150" x14ac:dyDescent="0.25">
@@ -3840,7 +3874,7 @@
         <v>236</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3854,7 +3888,7 @@
         <v>239</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3868,7 +3902,7 @@
         <v>242</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3882,7 +3916,7 @@
         <v>244</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,7 +3933,7 @@
         <v>23</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3914,7 +3948,7 @@
       </c>
       <c r="D143" s="3"/>
       <c r="E143" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3929,7 +3963,7 @@
       </c>
       <c r="D144" s="5"/>
       <c r="E144" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3944,7 +3978,7 @@
       </c>
       <c r="D145" s="5"/>
       <c r="E145" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3971,7 +4005,7 @@
       </c>
       <c r="D147" s="5"/>
       <c r="E147" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3986,7 +4020,7 @@
       </c>
       <c r="D148" s="5"/>
       <c r="E148" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4025,10 +4059,10 @@
       </c>
       <c r="D151" s="5"/>
       <c r="E151" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>33</v>
       </c>
@@ -4040,7 +4074,7 @@
       </c>
       <c r="D152" s="5"/>
       <c r="E152" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4067,7 +4101,7 @@
       </c>
       <c r="D154" s="5"/>
       <c r="E154" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4104,7 +4138,7 @@
       </c>
       <c r="D157" s="5"/>
       <c r="E157" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4119,7 +4153,7 @@
       </c>
       <c r="D158" s="5"/>
       <c r="E158" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4134,7 +4168,7 @@
       </c>
       <c r="D159" s="5"/>
       <c r="E159" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4149,7 +4183,7 @@
       </c>
       <c r="D160" s="5"/>
       <c r="E160" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -4164,7 +4198,7 @@
       </c>
       <c r="D161" s="5"/>
       <c r="E161" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4179,7 +4213,7 @@
       </c>
       <c r="D162" s="5"/>
       <c r="E162" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4194,7 +4228,7 @@
       </c>
       <c r="D163" s="5"/>
       <c r="E163" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4209,7 +4243,7 @@
       </c>
       <c r="D164" s="5"/>
       <c r="E164" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4224,7 +4258,7 @@
       </c>
       <c r="D165" s="5"/>
       <c r="E165" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -4239,7 +4273,7 @@
       </c>
       <c r="D166" s="5"/>
       <c r="E166" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4254,7 +4288,7 @@
       </c>
       <c r="D167" s="5"/>
       <c r="E167" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4269,7 +4303,7 @@
       </c>
       <c r="D168" s="5"/>
       <c r="E168" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -4286,7 +4320,7 @@
         <v>297</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4301,7 +4335,7 @@
       </c>
       <c r="D170" s="5"/>
       <c r="E170" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,7 +4350,7 @@
       </c>
       <c r="D171" s="5"/>
       <c r="E171" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4331,7 +4365,7 @@
       </c>
       <c r="D172" s="5"/>
       <c r="E172" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4346,7 +4380,7 @@
       </c>
       <c r="D173" s="5"/>
       <c r="E173" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4361,7 +4395,7 @@
       </c>
       <c r="D174" s="5"/>
       <c r="E174" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4376,7 +4410,7 @@
       </c>
       <c r="D175" s="5"/>
       <c r="E175" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4391,7 +4425,7 @@
       </c>
       <c r="D176" s="5"/>
       <c r="E176" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4406,7 +4440,7 @@
       </c>
       <c r="D177" s="5"/>
       <c r="E177" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4421,7 +4455,7 @@
       </c>
       <c r="D178" s="5"/>
       <c r="E178" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4436,7 +4470,7 @@
       </c>
       <c r="D179" s="5"/>
       <c r="E179" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4451,7 +4485,7 @@
       </c>
       <c r="D180" s="5"/>
       <c r="E180" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4466,7 +4500,7 @@
       </c>
       <c r="D181" s="5"/>
       <c r="E181" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4481,7 +4515,7 @@
       </c>
       <c r="D182" s="3"/>
       <c r="E182" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4496,7 +4530,7 @@
       </c>
       <c r="D183" s="3"/>
       <c r="E183" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4511,7 +4545,7 @@
       </c>
       <c r="D184" s="3"/>
       <c r="E184" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4526,7 +4560,7 @@
       </c>
       <c r="D185" s="3"/>
       <c r="E185" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4541,7 +4575,7 @@
       </c>
       <c r="D186" s="3"/>
       <c r="E186" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4556,7 +4590,7 @@
       </c>
       <c r="D187" s="3"/>
       <c r="E187" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4571,7 +4605,7 @@
       </c>
       <c r="D188" s="3"/>
       <c r="E188" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -4586,7 +4620,7 @@
       </c>
       <c r="D189" s="3"/>
       <c r="E189" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -4600,7 +4634,7 @@
         <v>286</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4614,7 +4648,7 @@
         <v>286</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4628,7 +4662,7 @@
         <v>333</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4642,7 +4676,7 @@
         <v>335</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4656,7 +4690,7 @@
         <v>337</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4670,7 +4704,7 @@
         <v>311</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4684,7 +4718,7 @@
         <v>340</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4698,7 +4732,7 @@
         <v>342</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4712,7 +4746,7 @@
         <v>322</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4726,7 +4760,7 @@
         <v>322</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4740,7 +4774,7 @@
         <v>322</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4754,7 +4788,7 @@
         <v>347</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4768,7 +4802,7 @@
         <v>349</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4782,7 +4816,7 @@
         <v>276</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -4796,7 +4830,7 @@
         <v>286</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -4810,7 +4844,7 @@
         <v>286</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -4824,7 +4858,7 @@
         <v>353</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -4838,7 +4872,7 @@
         <v>355</v>
       </c>
       <c r="E207" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -4852,7 +4886,7 @@
         <v>337</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -4866,7 +4900,7 @@
         <v>358</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -4880,7 +4914,7 @@
         <v>360</v>
       </c>
       <c r="E210" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4894,7 +4928,7 @@
         <v>362</v>
       </c>
       <c r="E211" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4907,6 +4941,9 @@
       <c r="C212" s="5" t="s">
         <v>364</v>
       </c>
+      <c r="E212" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
@@ -4918,6 +4955,9 @@
       <c r="C213" s="5" t="s">
         <v>286</v>
       </c>
+      <c r="E213" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
@@ -4929,6 +4969,9 @@
       <c r="C214" s="5" t="s">
         <v>337</v>
       </c>
+      <c r="E214" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
@@ -4940,6 +4983,9 @@
       <c r="C215" s="5" t="s">
         <v>368</v>
       </c>
+      <c r="E215" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
@@ -4951,6 +4997,9 @@
       <c r="C216" s="5" t="s">
         <v>370</v>
       </c>
+      <c r="E216" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
@@ -4962,6 +5011,9 @@
       <c r="C217" s="5" t="s">
         <v>337</v>
       </c>
+      <c r="E217" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
@@ -4973,6 +5025,9 @@
       <c r="C218" s="5" t="s">
         <v>373</v>
       </c>
+      <c r="E218" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
@@ -4984,6 +5039,9 @@
       <c r="C219" s="3" t="s">
         <v>373</v>
       </c>
+      <c r="E219" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
@@ -4995,6 +5053,9 @@
       <c r="C220" s="5" t="s">
         <v>373</v>
       </c>
+      <c r="E220" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
@@ -5006,6 +5067,9 @@
       <c r="C221" s="5" t="s">
         <v>376</v>
       </c>
+      <c r="E221" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
@@ -5017,6 +5081,9 @@
       <c r="C222" s="5" t="s">
         <v>286</v>
       </c>
+      <c r="E222" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
@@ -5028,6 +5095,9 @@
       <c r="C223" s="5" t="s">
         <v>379</v>
       </c>
+      <c r="E223" s="6" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
@@ -5039,8 +5109,11 @@
       <c r="C224" s="5" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>56</v>
       </c>
@@ -5050,8 +5123,11 @@
       <c r="C225" s="5" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>56</v>
       </c>
@@ -5061,8 +5137,11 @@
       <c r="C226" s="5" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E226" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>57</v>
       </c>
@@ -5072,8 +5151,11 @@
       <c r="C227" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>57</v>
       </c>
@@ -5083,8 +5165,11 @@
       <c r="C228" s="5" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>58</v>
       </c>
@@ -5094,8 +5179,11 @@
       <c r="C229" s="5" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>52</v>
       </c>
@@ -5105,8 +5193,11 @@
       <c r="C230" s="5" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E230" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>58</v>
       </c>
@@ -5116,8 +5207,11 @@
       <c r="C231" s="5" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>58</v>
       </c>
@@ -5127,8 +5221,11 @@
       <c r="C232" s="5" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E232" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>58</v>
       </c>
@@ -5138,8 +5235,11 @@
       <c r="C233" s="5" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
         <v>0</v>
       </c>
@@ -5152,8 +5252,11 @@
       <c r="D234" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E234" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A235" s="6">
         <v>60</v>
       </c>
@@ -5164,8 +5267,11 @@
         <v>394</v>
       </c>
       <c r="D235" s="8"/>
-    </row>
-    <row r="236" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E235" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="6">
         <v>60</v>
       </c>
@@ -5176,8 +5282,11 @@
         <v>396</v>
       </c>
       <c r="D236" s="8"/>
-    </row>
-    <row r="237" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E236" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="6">
         <v>60</v>
       </c>
@@ -5188,8 +5297,11 @@
         <v>398</v>
       </c>
       <c r="D237" s="8"/>
-    </row>
-    <row r="238" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E237" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="6">
         <v>60</v>
       </c>
@@ -5200,8 +5312,11 @@
         <v>400</v>
       </c>
       <c r="D238" s="8"/>
-    </row>
-    <row r="239" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E238" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A239" s="6">
         <v>84</v>
       </c>
@@ -5212,8 +5327,11 @@
         <v>402</v>
       </c>
       <c r="D239" s="8"/>
-    </row>
-    <row r="240" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E239" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A240" s="6">
         <v>62</v>
       </c>
@@ -5224,8 +5342,11 @@
         <v>404</v>
       </c>
       <c r="D240" s="8"/>
-    </row>
-    <row r="241" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E240" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="6">
         <v>62</v>
       </c>
@@ -5236,8 +5357,11 @@
         <v>405</v>
       </c>
       <c r="D241" s="8"/>
-    </row>
-    <row r="242" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E241" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="6">
         <v>62</v>
       </c>
@@ -5248,8 +5372,11 @@
         <v>406</v>
       </c>
       <c r="D242" s="8"/>
-    </row>
-    <row r="243" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E242" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" s="6">
         <v>63</v>
       </c>
@@ -5260,8 +5387,11 @@
         <v>408</v>
       </c>
       <c r="D243" s="8"/>
-    </row>
-    <row r="244" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E243" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="6">
         <v>63</v>
       </c>
@@ -5270,8 +5400,11 @@
       </c>
       <c r="C244" s="8"/>
       <c r="D244" s="8"/>
-    </row>
-    <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E244" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="6">
         <v>63</v>
       </c>
@@ -5282,8 +5415,11 @@
         <v>411</v>
       </c>
       <c r="D245" s="8"/>
-    </row>
-    <row r="246" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E245" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="6">
         <v>63</v>
       </c>
@@ -5293,7 +5429,7 @@
       <c r="C246" s="8"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A247" s="6">
         <v>63</v>
       </c>
@@ -5304,8 +5440,11 @@
         <v>414</v>
       </c>
       <c r="D247" s="8"/>
-    </row>
-    <row r="248" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E247" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="6">
         <v>63</v>
       </c>
@@ -5316,8 +5455,11 @@
         <v>416</v>
       </c>
       <c r="D248" s="8"/>
-    </row>
-    <row r="249" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E248" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A249" s="6">
         <v>63</v>
       </c>
@@ -5328,8 +5470,11 @@
         <v>417</v>
       </c>
       <c r="D249" s="8"/>
-    </row>
-    <row r="250" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E249" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A250" s="6">
         <v>63</v>
       </c>
@@ -5340,8 +5485,11 @@
         <v>419</v>
       </c>
       <c r="D250" s="8"/>
-    </row>
-    <row r="251" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E250" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A251" s="6">
         <v>30</v>
       </c>
@@ -5354,8 +5502,11 @@
       <c r="D251" s="8" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" ht="315" x14ac:dyDescent="0.25">
+      <c r="E251" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
         <v>422</v>
       </c>
@@ -5368,8 +5519,11 @@
       <c r="D252" s="8" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E252" s="8" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A253" s="6">
         <v>63</v>
       </c>
@@ -5378,8 +5532,11 @@
       </c>
       <c r="C253" s="8"/>
       <c r="D253" s="8"/>
-    </row>
-    <row r="254" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E253" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="6">
         <v>64</v>
       </c>
@@ -5390,8 +5547,11 @@
         <v>428</v>
       </c>
       <c r="D254" s="8"/>
-    </row>
-    <row r="255" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E254" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A255" s="6">
         <v>64</v>
       </c>
@@ -5402,8 +5562,11 @@
         <v>430</v>
       </c>
       <c r="D255" s="8"/>
-    </row>
-    <row r="256" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E255" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="6">
         <v>61</v>
       </c>
@@ -5414,8 +5577,11 @@
         <v>432</v>
       </c>
       <c r="D256" s="8"/>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E256" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="6">
         <v>64</v>
       </c>
@@ -5426,8 +5592,11 @@
         <v>434</v>
       </c>
       <c r="D257" s="8"/>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E257" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A258" s="6">
         <v>64</v>
       </c>
@@ -5435,11 +5604,11 @@
         <v>435</v>
       </c>
       <c r="C258" s="8" t="s">
-        <v>436</v>
+        <v>529</v>
       </c>
       <c r="D258" s="8"/>
     </row>
-    <row r="259" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A259" s="6">
         <v>64</v>
       </c>
@@ -5447,417 +5616,493 @@
         <v>435</v>
       </c>
       <c r="C259" s="8" t="s">
-        <v>437</v>
+        <v>530</v>
       </c>
       <c r="D259" s="8"/>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E259" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="6">
         <v>65</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C260" s="8" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D260" s="8"/>
-    </row>
-    <row r="261" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E260" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="6">
         <v>65</v>
       </c>
       <c r="B261" s="8" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C261" s="8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D261" s="8"/>
-    </row>
-    <row r="262" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E261" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="6">
         <v>65</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C262" s="8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D262" s="8"/>
-    </row>
-    <row r="263" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E262" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" s="6">
         <v>81</v>
       </c>
       <c r="B263" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C263" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="C263" s="8" t="s">
-        <v>444</v>
-      </c>
       <c r="D263" s="8"/>
-    </row>
-    <row r="264" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E263" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="6">
         <v>66</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C264" s="8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D264" s="8"/>
-    </row>
-    <row r="265" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E264" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A265" s="6">
         <v>66</v>
       </c>
       <c r="B265" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C265" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="D265" s="8"/>
+    </row>
+    <row r="266" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A266" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B266" s="8" t="s">
         <v>447</v>
-      </c>
-      <c r="C265" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="D265" s="8"/>
-    </row>
-    <row r="266" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A266" s="6" t="s">
-        <v>449</v>
-      </c>
-      <c r="B266" s="8" t="s">
-        <v>450</v>
       </c>
       <c r="C266" s="8"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C267" s="8"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A268" s="6">
         <v>66</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C268" s="8"/>
       <c r="D268" s="8"/>
-    </row>
-    <row r="269" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E268" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="6">
         <v>66</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C269" s="8" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D269" s="8"/>
     </row>
-    <row r="270" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A270" s="6">
         <v>65</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="C270" s="6"/>
+        <v>452</v>
+      </c>
+      <c r="C270" s="8" t="s">
+        <v>538</v>
+      </c>
       <c r="D270" s="8"/>
     </row>
-    <row r="271" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="8" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C271" s="8"/>
       <c r="D271" s="8"/>
-    </row>
-    <row r="272" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E271" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A272" s="8" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B272" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="C272" s="8"/>
+        <v>456</v>
+      </c>
+      <c r="C272" s="8" t="s">
+        <v>534</v>
+      </c>
       <c r="D272" s="8"/>
     </row>
-    <row r="273" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A273" s="8">
         <v>67</v>
       </c>
       <c r="B273" s="8" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C273" s="8" t="s">
-        <v>461</v>
+        <v>535</v>
       </c>
       <c r="D273" s="8"/>
-    </row>
-    <row r="274" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E273" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A274" s="8">
         <v>67</v>
       </c>
       <c r="B274" s="8" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C274" s="8" t="s">
-        <v>462</v>
+        <v>536</v>
       </c>
       <c r="D274" s="8"/>
     </row>
-    <row r="275" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="8">
         <v>67</v>
       </c>
       <c r="B275" s="8" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C275" s="8" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D275" s="8"/>
-    </row>
-    <row r="276" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E275" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A276" s="8">
         <v>67</v>
       </c>
       <c r="B276" s="8" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C276" s="8" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D276" s="8"/>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E276" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="8">
         <v>67</v>
       </c>
       <c r="B277" s="8" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C277" s="8" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D277" s="8"/>
-    </row>
-    <row r="278" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E277" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A278" s="8">
         <v>67</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C278" s="8" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D278" s="8"/>
     </row>
-    <row r="279" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="8">
         <v>67</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C279" s="8" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D279" s="8"/>
-    </row>
-    <row r="280" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E279" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A280" s="8">
         <v>68</v>
       </c>
       <c r="B280" s="8" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C280" s="8" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D280" s="8"/>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E280" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="8">
         <v>68</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C281" s="8" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D281" s="8"/>
     </row>
-    <row r="282" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>68</v>
       </c>
       <c r="B282" s="8" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C282" s="8" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D282" s="8"/>
     </row>
-    <row r="283" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A283" s="8">
         <v>68</v>
       </c>
       <c r="B283" s="8" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C283" s="8" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D283" s="8"/>
     </row>
-    <row r="284" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A284" s="8">
         <v>68</v>
       </c>
       <c r="B284" s="8" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C284" s="8" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D284" s="8"/>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="8">
         <v>68</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C285" s="8" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D285" s="8"/>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E285" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="8">
         <v>68</v>
       </c>
       <c r="B286" s="8" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C286" s="8" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D286" s="8"/>
-    </row>
-    <row r="287" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E286" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A287" s="8">
         <v>69</v>
       </c>
       <c r="B287" s="8" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C287" s="8" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D287" s="8"/>
-    </row>
-    <row r="288" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E287" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="8">
         <v>69</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C288" s="8" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D288" s="8"/>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E288" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="8">
         <v>70</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C289" s="8" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D289" s="8"/>
-    </row>
-    <row r="290" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E289" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="8">
         <v>70</v>
       </c>
       <c r="B290" s="8" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="C290" s="8" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="D290" s="8"/>
-    </row>
-    <row r="291" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E290" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A291" s="8">
         <v>70</v>
       </c>
       <c r="B291" s="8" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="C291" s="8" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D291" s="8"/>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E291" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="8">
         <v>70</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C292" s="8" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D292" s="8"/>
-    </row>
-    <row r="293" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E292" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="8">
         <v>71</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="C293" s="8"/>
       <c r="D293" s="8"/>
-    </row>
-    <row r="294" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E293" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="8">
         <v>80</v>
       </c>
       <c r="B294" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C294" s="8" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D294" s="8"/>
-    </row>
-    <row r="295" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E294" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="8">
         <v>80</v>
       </c>
@@ -5865,247 +6110,310 @@
         <v>285</v>
       </c>
       <c r="C295" s="8" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D295" s="8"/>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="8">
         <v>80</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C296" s="8" t="s">
         <v>337</v>
       </c>
       <c r="D296" s="8"/>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E296" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="6">
         <v>52</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C297" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D297" s="8"/>
-    </row>
-    <row r="298" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E297" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="8">
         <v>81</v>
       </c>
       <c r="B298" s="8" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C298" s="8" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D298" s="8"/>
-    </row>
-    <row r="299" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E298" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A299" s="8">
         <v>81</v>
       </c>
       <c r="B299" s="8" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C299" s="8" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D299" s="8"/>
-    </row>
-    <row r="300" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E299" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" s="8">
         <v>82</v>
       </c>
       <c r="B300" s="8" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C300" s="8"/>
       <c r="D300" s="8"/>
-    </row>
-    <row r="301" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E300" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A301" s="8">
         <v>82</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C301" s="8"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A302" s="8">
         <v>66</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="C302" s="8"/>
+        <v>503</v>
+      </c>
+      <c r="C302" s="8" t="s">
+        <v>537</v>
+      </c>
       <c r="D302" s="8"/>
-    </row>
-    <row r="303" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E302" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A303" s="8">
         <v>83</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C303" s="8"/>
       <c r="D303" s="8"/>
-    </row>
-    <row r="304" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E303" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A304" s="8">
         <v>85</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C304" s="8"/>
       <c r="D304" s="8"/>
-    </row>
-    <row r="305" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E304" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A305" s="8">
         <v>86</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="C305" s="8"/>
       <c r="D305" s="8"/>
-    </row>
-    <row r="306" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E305" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A306" s="8">
         <v>86</v>
       </c>
       <c r="B306" s="8" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C306" s="8"/>
       <c r="D306" s="8"/>
-    </row>
-    <row r="307" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E306" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A307" s="8">
         <v>86</v>
       </c>
       <c r="B307" s="8" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C307" s="8"/>
       <c r="D307" s="8"/>
-    </row>
-    <row r="308" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E307" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A308" s="8">
         <v>85</v>
       </c>
       <c r="B308" s="8" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="C308" s="8"/>
       <c r="D308" s="8"/>
-    </row>
-    <row r="309" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E308" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A309" s="8">
         <v>85</v>
       </c>
       <c r="B309" s="8" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C309" s="8"/>
       <c r="D309" s="8"/>
-    </row>
-    <row r="310" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="E309" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A310" s="8">
         <v>86</v>
       </c>
       <c r="B310" s="8" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="C310" s="8"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B311" s="8" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="C311" s="8"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B312" s="8" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C312" s="8"/>
       <c r="D312" s="8"/>
-    </row>
-    <row r="313" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E312" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
         <v>209</v>
       </c>
       <c r="B313" s="8" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C313" s="8"/>
       <c r="D313" s="8"/>
-    </row>
-    <row r="314" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E313" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="C314" s="8"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C315" s="8"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="C316" s="8"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A317" s="5"/>
-      <c r="B317" s="8"/>
-      <c r="C317" s="8"/>
+    <row r="317" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A317" s="5">
+        <v>60</v>
+      </c>
+      <c r="B317" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="C317" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="D317" s="8"/>
-    </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A318" s="5"/>
-      <c r="B318" s="8"/>
+      <c r="E317" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A318" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B318" s="8" t="s">
+        <v>526</v>
+      </c>
       <c r="C318" s="8"/>
       <c r="D318" s="8"/>
-    </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E318" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="5"/>
       <c r="B319" s="8"/>
       <c r="C319" s="8"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="5"/>
       <c r="B320" s="8"/>
       <c r="C320" s="8"/>

</xml_diff>

<commit_message>
Fixed discrepancies, typos, probably changed two weapon fighting again. Added some new issues. Closed many, many more.
</commit_message>
<xml_diff>
--- a/TODO/Proofreading.xlsx
+++ b/TODO/Proofreading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="543">
   <si>
     <t>Page</t>
   </si>
@@ -1641,6 +1641,18 @@
   </si>
   <si>
     <t>We break our alphabetization here, and then repeat some things. I don't care how, but we should clean this up</t>
+  </si>
+  <si>
+    <t>Teleport random spacing</t>
+  </si>
+  <si>
+    <t>Glossary isn't alphabetized, and there is weird, inconsistent spacing between items</t>
+  </si>
+  <si>
+    <t>86 ish</t>
+  </si>
+  <si>
+    <t>There's also this gross thing going on between rest, short rest, encounter, day, extended rest that should be cleaned up. I think it's important to leave to concepts of encoutner and day, I don't think it's important to stress the 24 hour bit. I also don't think extended rest should redirect to day, I think it should perhaps be the inverse. Honestly, Rest is a nice middle ground, but it's in the wrong place.</t>
   </si>
 </sst>
 </file>
@@ -2008,8 +2020,8 @@
   <dimension ref="A1:E721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E310" sqref="E310"/>
+      <pane ySplit="1" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C321" sqref="C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6408,15 +6420,28 @@
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A319" s="5"/>
-      <c r="B319" s="8"/>
+      <c r="A319" s="5">
+        <v>86</v>
+      </c>
+      <c r="B319" s="8" t="s">
+        <v>539</v>
+      </c>
       <c r="C319" s="8"/>
       <c r="D319" s="8"/>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A320" s="5"/>
-      <c r="B320" s="8"/>
-      <c r="C320" s="8"/>
+      <c r="E319" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A320" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="C320" s="8" t="s">
+        <v>542</v>
+      </c>
       <c r="D320" s="8"/>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>